<commit_message>
Update Indeed Data Scraping - PHP Developer and Python Developer
</commit_message>
<xml_diff>
--- a/data_result/Python Developer.xlsx
+++ b/data_result/Python Developer.xlsx
@@ -470,68 +470,68 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Full Stack Developer E-Commerce</t>
+          <t>Data Warehouse Engineer</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Kompas Gramedia</t>
+          <t>GO-JEK</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/Kompas-Gramedia-Group</t>
+          <t>https://id.indeed.com//cmp/Pt.-Go--jek-Indonesia-2</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Software Quality Assurance Intern</t>
+          <t>Lead Instructors - Le Wagon Data Science Bootcamp</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Shopee</t>
+          <t>Le Wagon Bali</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/Shopee</t>
+          <t>Link is not available</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>BaruQA Engineer</t>
+          <t>ShopeePay Backend Engineer [Experienced]</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>StyleTheory</t>
+          <t>Shopee</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/Styletheory</t>
+          <t>https://id.indeed.com//cmp/Shopee</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>ShopeePay Backend Engineer [Experienced]</t>
+          <t>Back End Developer</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Shopee</t>
+          <t>PT Generasi Teknologi Buana</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/Shopee</t>
+          <t>Link is not available</t>
         </is>
       </c>
     </row>
@@ -555,46 +555,46 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Data Warehouse Engineer</t>
+          <t>Associate Backend Engineer</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>GO-JEK</t>
+          <t>KeDA Tech</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/Pt.-Go--jek-Indonesia-2</t>
+          <t>Link is not available</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Associate Backend Engineer</t>
+          <t>QA Engineer</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>KeDA Tech</t>
+          <t>StyleTheory</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Link is not available</t>
+          <t>https://id.indeed.com//cmp/Styletheory</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Back End Developer</t>
+          <t>Developer / Programmer</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>PT Generasi Teknologi Buana</t>
+          <t>StrategArt</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -606,29 +606,29 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Blockchain Developer</t>
+          <t>Back End Developer - Kompas.id</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>PT. Inti Artistika Solusitama</t>
+          <t>Kompas Gramedia</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Link is not available</t>
+          <t>https://id.indeed.com//cmp/Kompas-Gramedia-Group</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Product Support Engineer</t>
+          <t>Back End Developer</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Awan Tunai</t>
+          <t>JULO</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -640,29 +640,29 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Senior Machine Learning</t>
+          <t>Python Junior Programmer</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Alodokter</t>
+          <t>Sonar Social Media Monitoring Platform</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/Alodokter-2</t>
+          <t>Link is not available</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Back End Developer</t>
+          <t>Problem Generator Developer</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>JULO</t>
+          <t>Zenius Education</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -674,29 +674,29 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Back End Developer - Kompas.id</t>
+          <t>Data Warehouse Engineer - GoPay</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Kompas Gramedia</t>
+          <t>GO-JEK</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/Kompas-Gramedia-Group</t>
+          <t>https://id.indeed.com//cmp/Pt.-Go--jek-Indonesia-2</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Developer / Programmer</t>
+          <t>Web Developer</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>StrategArt</t>
+          <t>Great Giant Foods</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -708,46 +708,46 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Web Developer</t>
+          <t>Application Developer</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>1rstWAP</t>
+          <t>Bank Mega</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Link is not available</t>
+          <t>https://id.indeed.com//cmp/Bank-Mega</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Business Intelligence Developer</t>
+          <t>Senior Machine Learning</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Stockbit-Bibit</t>
+          <t>Alodokter</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Link is not available</t>
+          <t>https://id.indeed.com//cmp/Alodokter-2</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Web Developer</t>
+          <t>Product Support Engineer</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Binabusana Internusa</t>
+          <t>Awan Tunai</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -759,29 +759,29 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>ShopeePay QA Engineer [Entry Level] - NEW</t>
+          <t>Software Engineer - Data Platform</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Shopee</t>
+          <t>Cermati.com</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/Shopee</t>
+          <t>https://id.indeed.com//cmp/PT-Dwi-Cermat-Indonesia-1</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Test Engineer</t>
+          <t>Project Manager / Jr. Project Manager / ERP Senior Consultan...</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Quipper</t>
+          <t>HashMicro</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -793,41 +793,41 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>BaruSoftware Engineer - Data Platform</t>
+          <t>Remote Senior Web Engineer</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Cermati.com</t>
+          <t>Scopic</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/PT-Dwi-Cermat-Indonesia-1</t>
+          <t>Link is not available</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>IT WEB DEVELOPER</t>
+          <t>HRIS Developer</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Ismaya Group</t>
+          <t>Binabusana Internusa</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/Ismaya-Group-1</t>
+          <t>Link is not available</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Financial Service SRE Engineer [Experienced]</t>
+          <t>Financial Service SRE Engineer [Entry Level]</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -844,46 +844,46 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Full Stack Developer E-Commerce</t>
+          <t>Web Developer</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Kompas Gramedia</t>
+          <t>1rstWAP</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/Kompas-Gramedia-Group</t>
+          <t>Link is not available</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Senior Machine Learning</t>
+          <t>Full Stack Developer</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Alodokter</t>
+          <t>Global Talentlytica</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/Alodokter-2</t>
+          <t>Link is not available</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>BaruETL Developer</t>
+          <t>Python Programmer</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Lawencon</t>
+          <t>1rstWAP</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -895,29 +895,29 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Senior Frontend Developer</t>
+          <t>Technical Solution Developer</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Ensoft</t>
+          <t>PT Mastersystem Infotama</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Link is not available</t>
+          <t>https://id.indeed.com//cmp/Pt.-Mastersystem-Infotama</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Associate Backend Engineer</t>
+          <t>Backend Developer</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>KeDA Tech</t>
+          <t>Pintek ID</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -929,46 +929,46 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Front End Development – Consultant</t>
+          <t>Test Engineer</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Accenture</t>
+          <t>Quipper</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/Accenture</t>
+          <t>Link is not available</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Back End Developer - Kompas.id</t>
+          <t>Engineering and Technology - Site Reliability Engineer</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Kompas Gramedia</t>
+          <t>Shopee</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/Kompas-Gramedia-Group</t>
+          <t>https://id.indeed.com//cmp/Shopee</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Tech Lead</t>
+          <t>Machine Learning Engineer</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Kasual</t>
+          <t>Nomura Research Institute Indonesia</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -980,46 +980,46 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Software Quality Assurance - Manual Testing</t>
+          <t>IT WEB DEVELOPER</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Indodana</t>
+          <t>Ismaya Group</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Link is not available</t>
+          <t>https://id.indeed.com//cmp/Ismaya-Group-1</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Technical Solution Developer</t>
+          <t>Back End Developer</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>PT Mastersystem Infotama</t>
+          <t>Akseleran</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/Pt.-Mastersystem-Infotama</t>
+          <t>Link is not available</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Blockchain Developer</t>
+          <t>Back End Developer</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>PT. Inti Artistika Solusitama</t>
+          <t>Renos.id</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1031,29 +1031,29 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Remote Senior Web Engineer</t>
+          <t>ShopeePay Backend Engineer [Leader]</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Scopic</t>
+          <t>Shopee</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Link is not available</t>
+          <t>https://id.indeed.com//cmp/Shopee</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Back End Developer</t>
+          <t>Web Developer</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>PT Generasi Teknologi Buana</t>
+          <t>Binabusana Internusa</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1065,29 +1065,29 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Software Quality Assurance - Manual Testing</t>
+          <t>IT Programmer Analyst</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Cermati.com</t>
+          <t>PT BSR Indonesia</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/PT-Dwi-Cermat-Indonesia-1</t>
+          <t>Link is not available</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Full Stack Developer</t>
+          <t>Golang Developer (Back End)</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>IndoSterling Technomedia</t>
+          <t>PT Lunaria Annua Teknologi (KoinWorks)</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1099,29 +1099,29 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>ShopeePay QA Engineer [Experienced]</t>
+          <t>Business Intelligence Developer E-Commerce</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Shopee</t>
+          <t>Kompas Gramedia</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/Shopee</t>
+          <t>https://id.indeed.com//cmp/Kompas-Gramedia-Group</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Back End Developer</t>
+          <t>IT Developer</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>JULO</t>
+          <t>MNC</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1133,131 +1133,131 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Backend Developer</t>
+          <t>Engineering and Technology - Back End Engineer, Payment Proc...</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Pintek ID</t>
+          <t>Shopee</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Link is not available</t>
+          <t>https://id.indeed.com//cmp/Shopee</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>QA Engineer - GoFinance</t>
+          <t>Senior Frontend Developer</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>GO-JEK</t>
+          <t>Ensoft</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/Pt.-Go--jek-Indonesia-2</t>
+          <t>Link is not available</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Business Intelligence Developer E-Commerce</t>
+          <t>Full Stack Developer</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Kompas Gramedia</t>
+          <t>IndoSterling Technomedia</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/Kompas-Gramedia-Group</t>
+          <t>Link is not available</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Senior Data Warehouse Engineer - GoPay</t>
+          <t>Test Engineer</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>GO-JEK</t>
+          <t>LINE Plus corporation</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/Pt.-Go--jek-Indonesia-2</t>
+          <t>Link is not available</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Full-Stack Developer</t>
+          <t>Senior Data Warehouse Engineer</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>DDTC</t>
+          <t>GO-JEK</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Link is not available</t>
+          <t>https://id.indeed.com//cmp/Pt.-Go--jek-Indonesia-2</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Fullstack Developer - Javascript, Python, Golang, NodeJS, Re...</t>
+          <t>Unity Developer</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Michael Page</t>
+          <t>Alegrium</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/Michael-Page</t>
+          <t>Link is not available</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Finance MIS Analyst - Financial Services</t>
+          <t>Test Engineer</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>GO-JEK</t>
+          <t>LINE Plus corporation</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/Pt.-Go--jek-Indonesia-2</t>
+          <t>Link is not available</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>IT Engineering Manager</t>
+          <t>Full-Stack Developer</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Ajaib</t>
+          <t>DDTC</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1269,80 +1269,80 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Problem Generator Developer</t>
+          <t>Software Quality Assurance - Manual Testing</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Zenius Education</t>
+          <t>Cermati.com</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Link is not available</t>
+          <t>https://id.indeed.com//cmp/PT-Dwi-Cermat-Indonesia-1</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Unity Developer</t>
+          <t>Senior Data Warehouse Engineer</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Alegrium</t>
+          <t>GO-JEK</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Link is not available</t>
+          <t>https://id.indeed.com//cmp/Pt.-Go--jek-Indonesia-2</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Engineer: Software Developer</t>
+          <t>Fullstack Developer - Javascript, Python, Golang, NodeJS, Re...</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>NTT Ltd</t>
+          <t>Michael Page</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Link is not available</t>
+          <t>https://id.indeed.com//cmp/Michael-Page</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>IT Developer</t>
+          <t>Customer Solutions Consultant, Infrastructure Modernization,...</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>MNC</t>
+          <t>Google</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Link is not available</t>
+          <t>https://id.indeed.com//cmp/Google</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Product Support Engineer</t>
+          <t>IT Engineering Manager</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Awan Tunai</t>
+          <t>Ajaib</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1354,12 +1354,12 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Test Engineer</t>
+          <t>System Administrator</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>LINE Plus corporation</t>
+          <t>Jawasoft</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1371,46 +1371,46 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Senior Data Warehouse Engineer</t>
+          <t>IT Developer</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>GO-JEK</t>
+          <t>MNC</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/Pt.-Go--jek-Indonesia-2</t>
+          <t>Link is not available</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Customer Solutions Consultant, Infrastructure Modernization,...</t>
+          <t>Engineer: Software Developer</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Google</t>
+          <t>NTT Ltd</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/Google</t>
+          <t>Link is not available</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Senior Software Engineer for Global AI Startup</t>
+          <t>Back End Developer</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>StrategArt</t>
+          <t>Renos.id</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -1422,114 +1422,114 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Product Owner (Entry, Mid and Senior Levels)</t>
+          <t>Software Developer</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Cermati.com</t>
+          <t>Terrindo Bumi Raya</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/PT-Dwi-Cermat-Indonesia-1</t>
+          <t>Link is not available</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Frontend Engineer (Freshgraduate, Senior, Principal, &amp; Senio...</t>
+          <t>Full Stack Developer</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Cermati.com</t>
+          <t>Global Talentlytica</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/PT-Dwi-Cermat-Indonesia-1</t>
+          <t>Link is not available</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>BaruSenior Software Engineer - Data Plarform</t>
+          <t>Senior Integration Developer</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Cermati.com</t>
+          <t>GO-JEK</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/PT-Dwi-Cermat-Indonesia-1</t>
+          <t>https://id.indeed.com//cmp/Pt.-Go--jek-Indonesia-2</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>System Administrator</t>
+          <t>Software Quality Assurance - Manual Testing</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Jawasoft</t>
+          <t>Cermati.com</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Link is not available</t>
+          <t>https://id.indeed.com//cmp/PT-Dwi-Cermat-Indonesia-1</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Solutions Architect - Developer Specialist</t>
+          <t>Technical Operations Engineer</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>PT Amazon Web Services IDN</t>
+          <t>byOrange</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/Amazon.com</t>
+          <t>Link is not available</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Back End Developer</t>
+          <t>Frontend Engineer (Freshgraduate, Senior, Principal, &amp; Senio...</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Renos.id</t>
+          <t>Cermati.com</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Link is not available</t>
+          <t>https://id.indeed.com//cmp/PT-Dwi-Cermat-Indonesia-1</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Senior/Software Engineer, Front End</t>
+          <t>(Singapore Corp) Python Software Developer</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Coda Payments</t>
+          <t>MatchaTalent</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -1541,12 +1541,12 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Software Engineer</t>
+          <t>IT Engineering Manager</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Alterra</t>
+          <t>Ajaib</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -1558,12 +1558,12 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Software Developer</t>
+          <t>System Administrator</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Terrindo Bumi Raya</t>
+          <t>Jawasoft</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -1575,7 +1575,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>BaruBackend Developer</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -1592,29 +1592,29 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Full Stack Developer</t>
+          <t>Financial Service SRE Engineer [Experienced]</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Global Talentlytica</t>
+          <t>Shopee</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Link is not available</t>
+          <t>https://id.indeed.com//cmp/Shopee</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Machine Learning Engineer</t>
+          <t>Software Engineer</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Nomura Research Institute Indonesia</t>
+          <t>Alterra</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -1626,46 +1626,46 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Golang Developer (Back End)</t>
+          <t>Finance MIS Analyst - Financial Services</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>PT Lunaria Annua Teknologi (KoinWorks)</t>
+          <t>GO-JEK</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Link is not available</t>
+          <t>https://id.indeed.com//cmp/Pt.-Go--jek-Indonesia-2</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Back End Developer</t>
+          <t>Back End Engineer</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Akseleran</t>
+          <t>Ruangguru</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Link is not available</t>
+          <t>https://id.indeed.com//cmp/PT-Ruang-Raya-Indonesia-(ruangguru)</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Assistant IT Project Manager</t>
+          <t>Server-side Engineer</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Simbadda Group</t>
+          <t>LINE Plus corporation</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -1677,51 +1677,51 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>IT Engineer</t>
+          <t>Unity Developer</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>PT Bank Central Asia Tbk</t>
+          <t>Alegrium</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/PT-Bank-Central-Asia-Tbk</t>
+          <t>Link is not available</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Back end developer</t>
+          <t>Engineering and Technology - System Quality Assurance</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>MNC</t>
+          <t>Shopee</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Link is not available</t>
+          <t>https://id.indeed.com//cmp/Shopee</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Remote) QA Engineer SDET</t>
+          <t>IT Engineer</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Kitabisa.com</t>
+          <t>PT Bank Central Asia Tbk</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Link is not available</t>
+          <t>https://id.indeed.com//cmp/PT-Bank-Central-Asia-Tbk</t>
         </is>
       </c>
     </row>

</xml_diff>